<commit_message>
fragility_data.damage_median renamed too fragility_data.median in all model.json, all model.xlsx and code base. fragility_data.damage_logstd renamed too fragility_data.beta  in all model.json, all model.xlsx and code base. test cases adjusted to change. All hard coded constant relating to algorithms removed.
</commit_message>
<xml_diff>
--- a/models/powerstation_coal/sysconfig_pscoal_identical_comps.xlsx
+++ b/models/powerstation_coal/sysconfig_pscoal_identical_comps.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="465" windowWidth="28695" windowHeight="16845" tabRatio="804"/>
+    <workbookView xWindow="0" yWindow="465" windowWidth="28695" windowHeight="16845" tabRatio="804" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="table_description" sheetId="11" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1763" uniqueCount="266">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1763" uniqueCount="267">
   <si>
     <t>pwr_house</t>
   </si>
@@ -606,9 +606,6 @@
     <t>component_id</t>
   </si>
   <si>
-    <t>damage_median</t>
-  </si>
-  <si>
     <t>Capacity at the output nodes on the extremity of the component network</t>
   </si>
   <si>
@@ -826,6 +823,12 @@
   </si>
   <si>
     <t>damage_state_def</t>
+  </si>
+  <si>
+    <t>median</t>
+  </si>
+  <si>
+    <t>beta</t>
   </si>
 </sst>
 </file>
@@ -2845,7 +2848,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G15" sqref="G15"/>
     </sheetView>
   </sheetViews>
@@ -2853,51 +2856,51 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>252</v>
+      </c>
+      <c r="B1" t="s">
         <v>253</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>254</v>
-      </c>
-      <c r="C1" t="s">
-        <v>255</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>255</v>
+      </c>
+      <c r="B2" t="s">
         <v>256</v>
       </c>
-      <c r="B2" t="s">
+      <c r="C2" t="s">
         <v>257</v>
-      </c>
-      <c r="C2" t="s">
-        <v>258</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
+        <v>258</v>
+      </c>
+      <c r="B3" t="s">
+        <v>215</v>
+      </c>
+      <c r="C3" t="s">
         <v>259</v>
-      </c>
-      <c r="B3" t="s">
-        <v>216</v>
-      </c>
-      <c r="C3" t="s">
-        <v>260</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="B4" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="C4" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="B5" t="s">
         <v>9</v>
@@ -2908,21 +2911,21 @@
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="B6" t="s">
         <v>155</v>
       </c>
       <c r="C6" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="B7" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
     </row>
   </sheetData>
@@ -5278,22 +5281,22 @@
     </row>
     <row r="2" spans="1:7" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="72" t="s">
+        <v>208</v>
+      </c>
+      <c r="B2" s="72" t="s">
         <v>209</v>
       </c>
-      <c r="B2" s="72" t="s">
-        <v>210</v>
-      </c>
       <c r="C2" s="59" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="D2" s="73">
         <v>0</v>
       </c>
       <c r="E2" s="74" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="F2" s="72" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="G2" s="75">
         <v>1</v>
@@ -5301,13 +5304,13 @@
     </row>
     <row r="3" spans="1:7" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="59" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="B3" s="59" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="C3" s="59" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="D3" s="73">
         <v>2.5954017126034994E-2</v>
@@ -5316,7 +5319,7 @@
         <v>16</v>
       </c>
       <c r="F3" s="72" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="G3" s="75">
         <v>1</v>
@@ -5324,13 +5327,13 @@
     </row>
     <row r="4" spans="1:7" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="59" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="B4" s="59" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="C4" s="59" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="D4" s="73">
         <v>2.5954017126034994E-2</v>
@@ -5339,7 +5342,7 @@
         <v>16</v>
       </c>
       <c r="F4" s="72" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="G4" s="75">
         <v>1</v>
@@ -5350,10 +5353,10 @@
         <v>10</v>
       </c>
       <c r="B5" s="59" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="C5" s="59" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="D5" s="106">
         <v>0.01</v>
@@ -5362,7 +5365,7 @@
         <v>16</v>
       </c>
       <c r="F5" s="72" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="G5" s="75">
         <v>1</v>
@@ -5373,7 +5376,7 @@
         <v>54</v>
       </c>
       <c r="B6" s="59" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="C6" s="59" t="s">
         <v>45</v>
@@ -5396,7 +5399,7 @@
         <v>55</v>
       </c>
       <c r="B7" s="59" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="C7" s="59" t="s">
         <v>45</v>
@@ -5419,7 +5422,7 @@
         <v>56</v>
       </c>
       <c r="B8" s="59" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="C8" s="59" t="s">
         <v>45</v>
@@ -5442,7 +5445,7 @@
         <v>29</v>
       </c>
       <c r="B9" s="59" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="C9" s="59" t="s">
         <v>46</v>
@@ -5465,7 +5468,7 @@
         <v>30</v>
       </c>
       <c r="B10" s="59" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="C10" s="59" t="s">
         <v>46</v>
@@ -5488,7 +5491,7 @@
         <v>31</v>
       </c>
       <c r="B11" s="59" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="C11" s="59" t="s">
         <v>46</v>
@@ -5511,7 +5514,7 @@
         <v>32</v>
       </c>
       <c r="B12" s="59" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="C12" s="59" t="s">
         <v>46</v>
@@ -5534,7 +5537,7 @@
         <v>1</v>
       </c>
       <c r="B13" s="59" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="C13" s="59" t="s">
         <v>47</v>
@@ -5557,7 +5560,7 @@
         <v>2</v>
       </c>
       <c r="B14" s="59" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="C14" s="59" t="s">
         <v>47</v>
@@ -5577,10 +5580,10 @@
     </row>
     <row r="15" spans="1:7" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="59" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="B15" s="59" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="C15" s="59" t="s">
         <v>44</v>
@@ -5589,7 +5592,7 @@
         <v>2.3189810486043766E-2</v>
       </c>
       <c r="E15" s="74" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="F15" s="59" t="s">
         <v>44</v>
@@ -5603,7 +5606,7 @@
         <v>11</v>
       </c>
       <c r="B16" s="59" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="C16" s="59" t="s">
         <v>44</v>
@@ -5626,7 +5629,7 @@
         <v>3</v>
       </c>
       <c r="B17" s="59" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="C17" s="59" t="s">
         <v>44</v>
@@ -5649,7 +5652,7 @@
         <v>4</v>
       </c>
       <c r="B18" s="59" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="C18" s="59" t="s">
         <v>44</v>
@@ -5672,7 +5675,7 @@
         <v>38</v>
       </c>
       <c r="B19" s="59" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="C19" s="59" t="s">
         <v>48</v>
@@ -5695,7 +5698,7 @@
         <v>39</v>
       </c>
       <c r="B20" s="59" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="C20" s="59" t="s">
         <v>48</v>
@@ -5718,7 +5721,7 @@
         <v>40</v>
       </c>
       <c r="B21" s="59" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="C21" s="59" t="s">
         <v>48</v>
@@ -5741,7 +5744,7 @@
         <v>41</v>
       </c>
       <c r="B22" s="59" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="C22" s="59" t="s">
         <v>48</v>
@@ -5764,10 +5767,10 @@
         <v>33</v>
       </c>
       <c r="B23" s="59" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="C23" s="59" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="D23" s="73">
         <v>4.9999999999999992E-3</v>
@@ -5776,7 +5779,7 @@
         <v>52</v>
       </c>
       <c r="F23" s="59" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="G23" s="75">
         <v>1</v>
@@ -5787,10 +5790,10 @@
         <v>5</v>
       </c>
       <c r="B24" s="59" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="C24" s="59" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="D24" s="73">
         <v>6.6793425473104144E-3</v>
@@ -5799,7 +5802,7 @@
         <v>16</v>
       </c>
       <c r="F24" s="59" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="G24" s="75">
         <v>1</v>
@@ -5810,10 +5813,10 @@
         <v>6</v>
       </c>
       <c r="B25" s="59" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="C25" s="59" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="D25" s="73">
         <v>6.6793425473104144E-3</v>
@@ -5822,7 +5825,7 @@
         <v>16</v>
       </c>
       <c r="F25" s="59" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="G25" s="75">
         <v>1</v>
@@ -5833,7 +5836,7 @@
         <v>0</v>
       </c>
       <c r="B26" s="59" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="C26" s="59" t="s">
         <v>51</v>
@@ -5845,7 +5848,7 @@
         <v>52</v>
       </c>
       <c r="F26" s="59" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="G26" s="75">
         <v>1</v>
@@ -5856,7 +5859,7 @@
         <v>57</v>
       </c>
       <c r="B27" s="59" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="C27" s="59" t="s">
         <v>42</v>
@@ -5879,7 +5882,7 @@
         <v>58</v>
       </c>
       <c r="B28" s="59" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="C28" s="59" t="s">
         <v>42</v>
@@ -5902,7 +5905,7 @@
         <v>7</v>
       </c>
       <c r="B29" s="59" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="C29" s="59" t="s">
         <v>51</v>
@@ -5925,7 +5928,7 @@
         <v>8</v>
       </c>
       <c r="B30" s="59" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="C30" s="59" t="s">
         <v>51</v>
@@ -5997,7 +6000,7 @@
         <v>28</v>
       </c>
       <c r="C33" s="59" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="D33" s="73">
         <v>0</v>
@@ -6006,7 +6009,7 @@
         <v>18</v>
       </c>
       <c r="F33" s="59" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="G33" s="75">
         <v>1</v>
@@ -6020,7 +6023,7 @@
         <v>28</v>
       </c>
       <c r="C34" s="59" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="D34" s="73">
         <v>0</v>
@@ -6029,7 +6032,7 @@
         <v>18</v>
       </c>
       <c r="F34" s="59" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="G34" s="75">
         <v>1</v>
@@ -6086,24 +6089,24 @@
   <sheetData>
     <row r="1" spans="1:4" ht="26.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="69" t="s">
+        <v>238</v>
+      </c>
+      <c r="B1" s="69" t="s">
         <v>239</v>
       </c>
-      <c r="B1" s="69" t="s">
+      <c r="C1" s="79" t="s">
+        <v>248</v>
+      </c>
+      <c r="D1" s="79" t="s">
         <v>240</v>
-      </c>
-      <c r="C1" s="79" t="s">
-        <v>249</v>
-      </c>
-      <c r="D1" s="79" t="s">
-        <v>241</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="59" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="B2" s="59" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="C2" s="80">
         <v>1</v>
@@ -6114,10 +6117,10 @@
     </row>
     <row r="3" spans="1:4" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="59" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="B3" s="59" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="C3" s="80">
         <v>1</v>
@@ -6128,7 +6131,7 @@
     </row>
     <row r="4" spans="1:4" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="59" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="B4" s="59" t="s">
         <v>10</v>
@@ -6142,7 +6145,7 @@
     </row>
     <row r="5" spans="1:4" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="59" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="B5" s="59" t="s">
         <v>10</v>
@@ -6394,7 +6397,7 @@
     </row>
     <row r="23" spans="1:4" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="59" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="B23" s="59" t="s">
         <v>11</v>
@@ -6714,21 +6717,21 @@
   <sheetData>
     <row r="1" spans="1:4" ht="26.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="60" t="s">
+        <v>241</v>
+      </c>
+      <c r="B1" s="61" t="s">
+        <v>243</v>
+      </c>
+      <c r="C1" s="61" t="s">
         <v>242</v>
       </c>
-      <c r="B1" s="61" t="s">
-        <v>244</v>
-      </c>
-      <c r="C1" s="61" t="s">
-        <v>243</v>
-      </c>
       <c r="D1" s="61" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="59" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="B2" s="62">
         <v>100</v>
@@ -6737,12 +6740,12 @@
         <v>1</v>
       </c>
       <c r="D2" s="64" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="65" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="B3" s="62">
         <v>100</v>
@@ -6751,7 +6754,7 @@
         <v>1</v>
       </c>
       <c r="D3" s="64" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
@@ -6801,19 +6804,19 @@
   <sheetData>
     <row r="1" spans="1:6" ht="26.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="60" t="s">
+        <v>244</v>
+      </c>
+      <c r="B1" s="60" t="s">
         <v>245</v>
       </c>
-      <c r="B1" s="60" t="s">
+      <c r="C1" s="61" t="s">
         <v>246</v>
       </c>
-      <c r="C1" s="61" t="s">
+      <c r="D1" s="61" t="s">
+        <v>242</v>
+      </c>
+      <c r="E1" s="61" t="s">
         <v>247</v>
-      </c>
-      <c r="D1" s="61" t="s">
-        <v>243</v>
-      </c>
-      <c r="E1" s="61" t="s">
-        <v>248</v>
       </c>
     </row>
     <row r="2" spans="1:6" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
@@ -6864,11 +6867,11 @@
   </sheetPr>
   <dimension ref="A1:O77"/>
   <sheetViews>
-    <sheetView zoomScale="115" zoomScaleNormal="115" zoomScalePageLayoutView="115" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" zoomScalePageLayoutView="115" workbookViewId="0">
       <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
-      <selection pane="bottomRight" sqref="A1:XFD3"/>
+      <selection pane="bottomRight" activeCell="H6" sqref="H6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="12.75" x14ac:dyDescent="0.25"/>
@@ -6895,16 +6898,16 @@
         <v>19</v>
       </c>
       <c r="C1" s="53" t="s">
+        <v>198</v>
+      </c>
+      <c r="D1" s="81" t="s">
         <v>199</v>
       </c>
-      <c r="D1" s="81" t="s">
-        <v>200</v>
-      </c>
       <c r="E1" s="89" t="s">
-        <v>192</v>
+        <v>265</v>
       </c>
       <c r="F1" s="89" t="s">
-        <v>20</v>
+        <v>266</v>
       </c>
       <c r="G1" s="89" t="s">
         <v>21</v>
@@ -6913,13 +6916,13 @@
         <v>22</v>
       </c>
       <c r="I1" s="87" t="s">
+        <v>202</v>
+      </c>
+      <c r="J1" s="87" t="s">
         <v>203</v>
       </c>
-      <c r="J1" s="87" t="s">
+      <c r="K1" s="87" t="s">
         <v>204</v>
-      </c>
-      <c r="K1" s="87" t="s">
-        <v>205</v>
       </c>
       <c r="L1" s="88" t="s">
         <v>23</v>
@@ -6928,7 +6931,7 @@
         <v>24</v>
       </c>
       <c r="N1" s="88" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="O1" s="108" t="s">
         <v>189</v>
@@ -6936,13 +6939,13 @@
     </row>
     <row r="2" spans="1:15" s="24" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="11" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="B2" s="11" t="s">
         <v>59</v>
       </c>
       <c r="C2" s="11" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="D2" s="83">
         <v>1</v>
@@ -6960,13 +6963,13 @@
         <v>1</v>
       </c>
       <c r="I2" s="85" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="J2" s="85" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="K2" s="85" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="L2" s="7">
         <v>5</v>
@@ -6984,13 +6987,13 @@
     </row>
     <row r="3" spans="1:15" s="24" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="10" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="B3" s="10" t="s">
         <v>60</v>
       </c>
       <c r="C3" s="10" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="D3" s="82">
         <v>1</v>
@@ -7008,13 +7011,13 @@
         <v>0</v>
       </c>
       <c r="I3" s="86" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="J3" s="86" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="K3" s="86" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="L3" s="9">
         <v>10</v>
@@ -7032,13 +7035,13 @@
     </row>
     <row r="4" spans="1:15" s="24" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="10" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="B4" s="10" t="s">
         <v>61</v>
       </c>
       <c r="C4" s="10" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="D4" s="82">
         <v>1</v>
@@ -7056,13 +7059,13 @@
         <v>0</v>
       </c>
       <c r="I4" s="86" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="J4" s="86" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="K4" s="86" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="L4" s="9">
         <v>21</v>
@@ -7080,13 +7083,13 @@
     </row>
     <row r="5" spans="1:15" s="24" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="10" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="B5" s="10" t="s">
         <v>62</v>
       </c>
       <c r="C5" s="10" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="D5" s="82">
         <v>1</v>
@@ -7104,13 +7107,13 @@
         <v>0</v>
       </c>
       <c r="I5" s="86" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="J5" s="86" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="K5" s="86" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="L5" s="52">
         <f>10*30/7</f>
@@ -7129,13 +7132,13 @@
     </row>
     <row r="6" spans="1:15" s="24" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" s="11" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="B6" s="11" t="s">
         <v>59</v>
       </c>
       <c r="C6" s="11" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="D6" s="83">
         <v>1</v>
@@ -7153,13 +7156,13 @@
         <v>1</v>
       </c>
       <c r="I6" s="85" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="J6" s="85" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="K6" s="85" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="L6" s="7">
         <v>5</v>
@@ -7175,13 +7178,13 @@
     </row>
     <row r="7" spans="1:15" s="24" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="10" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="B7" s="10" t="s">
         <v>60</v>
       </c>
       <c r="C7" s="10" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="D7" s="82">
         <v>1</v>
@@ -7199,13 +7202,13 @@
         <v>0</v>
       </c>
       <c r="I7" s="86" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="J7" s="86" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="K7" s="86" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="L7" s="9">
         <v>10</v>
@@ -7221,13 +7224,13 @@
     </row>
     <row r="8" spans="1:15" s="24" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8" s="10" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="B8" s="10" t="s">
         <v>61</v>
       </c>
       <c r="C8" s="10" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="D8" s="82">
         <v>1</v>
@@ -7245,13 +7248,13 @@
         <v>0</v>
       </c>
       <c r="I8" s="86" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="J8" s="86" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="K8" s="86" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="L8" s="9">
         <v>21</v>
@@ -7267,13 +7270,13 @@
     </row>
     <row r="9" spans="1:15" s="24" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="10" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="B9" s="10" t="s">
         <v>62</v>
       </c>
       <c r="C9" s="10" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="D9" s="82">
         <v>1</v>
@@ -7291,13 +7294,13 @@
         <v>0</v>
       </c>
       <c r="I9" s="86" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="J9" s="86" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="K9" s="86" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="L9" s="52">
         <f>10*30/7</f>
@@ -7314,13 +7317,13 @@
     </row>
     <row r="10" spans="1:15" s="43" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A10" s="11" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="B10" s="11" t="s">
         <v>59</v>
       </c>
       <c r="C10" s="11" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="D10" s="83">
         <v>1</v>
@@ -7338,13 +7341,13 @@
         <v>1</v>
       </c>
       <c r="I10" s="85" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="J10" s="85" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="K10" s="85" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="L10" s="7">
         <v>5</v>
@@ -7360,13 +7363,13 @@
     </row>
     <row r="11" spans="1:15" s="24" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A11" s="10" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="B11" s="10" t="s">
         <v>60</v>
       </c>
       <c r="C11" s="10" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="D11" s="82">
         <v>1</v>
@@ -7384,13 +7387,13 @@
         <v>0</v>
       </c>
       <c r="I11" s="86" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="J11" s="86" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="K11" s="86" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="L11" s="9">
         <v>10</v>
@@ -7406,13 +7409,13 @@
     </row>
     <row r="12" spans="1:15" s="24" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A12" s="10" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="B12" s="10" t="s">
         <v>61</v>
       </c>
       <c r="C12" s="10" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="D12" s="82">
         <v>1</v>
@@ -7430,13 +7433,13 @@
         <v>0</v>
       </c>
       <c r="I12" s="86" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="J12" s="86" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="K12" s="86" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="L12" s="9">
         <v>21</v>
@@ -7452,13 +7455,13 @@
     </row>
     <row r="13" spans="1:15" s="24" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A13" s="10" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="B13" s="10" t="s">
         <v>62</v>
       </c>
       <c r="C13" s="10" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="D13" s="82">
         <v>1</v>
@@ -7476,13 +7479,13 @@
         <v>0</v>
       </c>
       <c r="I13" s="86" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="J13" s="86" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="K13" s="86" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="L13" s="52">
         <f>10*30/7</f>
@@ -7499,13 +7502,13 @@
     </row>
     <row r="14" spans="1:15" s="24" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A14" s="11" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="B14" s="11" t="s">
         <v>59</v>
       </c>
       <c r="C14" s="11" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="D14" s="83">
         <v>1</v>
@@ -7523,13 +7526,13 @@
         <v>1</v>
       </c>
       <c r="I14" s="85" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="J14" s="85" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="K14" s="85" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="L14" s="7">
         <v>5</v>
@@ -7545,13 +7548,13 @@
     </row>
     <row r="15" spans="1:15" s="24" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A15" s="10" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="B15" s="10" t="s">
         <v>60</v>
       </c>
       <c r="C15" s="10" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="D15" s="82">
         <v>1</v>
@@ -7569,13 +7572,13 @@
         <v>0</v>
       </c>
       <c r="I15" s="86" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="J15" s="86" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="K15" s="86" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="L15" s="9">
         <v>10</v>
@@ -7591,13 +7594,13 @@
     </row>
     <row r="16" spans="1:15" s="24" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A16" s="10" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="B16" s="10" t="s">
         <v>61</v>
       </c>
       <c r="C16" s="10" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="D16" s="82">
         <v>1</v>
@@ -7615,13 +7618,13 @@
         <v>0</v>
       </c>
       <c r="I16" s="86" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="J16" s="86" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="K16" s="86" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="L16" s="9">
         <v>21</v>
@@ -7637,13 +7640,13 @@
     </row>
     <row r="17" spans="1:15" s="24" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A17" s="10" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="B17" s="10" t="s">
         <v>62</v>
       </c>
       <c r="C17" s="10" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="D17" s="82">
         <v>1</v>
@@ -7661,13 +7664,13 @@
         <v>0</v>
       </c>
       <c r="I17" s="86" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="J17" s="86" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="K17" s="86" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="L17" s="52">
         <f>10*30/7</f>
@@ -7684,13 +7687,13 @@
     </row>
     <row r="18" spans="1:15" s="24" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A18" s="11" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="B18" s="11" t="s">
         <v>59</v>
       </c>
       <c r="C18" s="11" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="D18" s="83">
         <v>1</v>
@@ -7708,13 +7711,13 @@
         <v>1</v>
       </c>
       <c r="I18" s="85" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="J18" s="85" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="K18" s="85" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="L18" s="7">
         <v>5</v>
@@ -7730,13 +7733,13 @@
     </row>
     <row r="19" spans="1:15" s="24" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A19" s="10" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="B19" s="10" t="s">
         <v>60</v>
       </c>
       <c r="C19" s="10" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="D19" s="82">
         <v>1</v>
@@ -7754,13 +7757,13 @@
         <v>0</v>
       </c>
       <c r="I19" s="86" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="J19" s="86" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="K19" s="86" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="L19" s="9">
         <v>10</v>
@@ -7776,13 +7779,13 @@
     </row>
     <row r="20" spans="1:15" s="24" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A20" s="10" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="B20" s="10" t="s">
         <v>61</v>
       </c>
       <c r="C20" s="10" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="D20" s="82">
         <v>1</v>
@@ -7800,13 +7803,13 @@
         <v>0</v>
       </c>
       <c r="I20" s="86" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="J20" s="86" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="K20" s="86" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="L20" s="9">
         <v>21</v>
@@ -7822,13 +7825,13 @@
     </row>
     <row r="21" spans="1:15" s="24" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A21" s="10" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="B21" s="10" t="s">
         <v>62</v>
       </c>
       <c r="C21" s="10" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="D21" s="82">
         <v>1</v>
@@ -7846,13 +7849,13 @@
         <v>0</v>
       </c>
       <c r="I21" s="86" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="J21" s="86" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="K21" s="86" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="L21" s="52">
         <f>10*30/7</f>
@@ -7869,13 +7872,13 @@
     </row>
     <row r="22" spans="1:15" s="24" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A22" s="11" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="B22" s="11" t="s">
         <v>59</v>
       </c>
       <c r="C22" s="11" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="D22" s="83">
         <v>1</v>
@@ -7893,13 +7896,13 @@
         <v>1</v>
       </c>
       <c r="I22" s="85" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="J22" s="85" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="K22" s="85" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="L22" s="7">
         <v>5</v>
@@ -7915,13 +7918,13 @@
     </row>
     <row r="23" spans="1:15" s="24" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A23" s="10" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="B23" s="10" t="s">
         <v>60</v>
       </c>
       <c r="C23" s="10" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="D23" s="82">
         <v>1</v>
@@ -7939,13 +7942,13 @@
         <v>0</v>
       </c>
       <c r="I23" s="86" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="J23" s="86" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="K23" s="86" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="L23" s="9">
         <v>10</v>
@@ -7961,13 +7964,13 @@
     </row>
     <row r="24" spans="1:15" s="24" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A24" s="10" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="B24" s="10" t="s">
         <v>61</v>
       </c>
       <c r="C24" s="10" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="D24" s="82">
         <v>1</v>
@@ -7985,13 +7988,13 @@
         <v>0</v>
       </c>
       <c r="I24" s="86" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="J24" s="86" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="K24" s="86" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="L24" s="9">
         <v>21</v>
@@ -8007,13 +8010,13 @@
     </row>
     <row r="25" spans="1:15" s="24" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A25" s="10" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="B25" s="10" t="s">
         <v>62</v>
       </c>
       <c r="C25" s="10" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="D25" s="82">
         <v>1</v>
@@ -8031,13 +8034,13 @@
         <v>0</v>
       </c>
       <c r="I25" s="86" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="J25" s="86" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="K25" s="86" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="L25" s="52">
         <f>10*30/7</f>
@@ -8054,13 +8057,13 @@
     </row>
     <row r="26" spans="1:15" s="24" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A26" s="11" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="B26" s="11" t="s">
         <v>59</v>
       </c>
       <c r="C26" s="11" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="D26" s="83">
         <v>1</v>
@@ -8078,13 +8081,13 @@
         <v>1</v>
       </c>
       <c r="I26" s="85" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="J26" s="85" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="K26" s="85" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="L26" s="7">
         <v>5</v>
@@ -8100,13 +8103,13 @@
     </row>
     <row r="27" spans="1:15" s="24" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A27" s="10" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="B27" s="10" t="s">
         <v>60</v>
       </c>
       <c r="C27" s="10" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="D27" s="82">
         <v>1</v>
@@ -8124,13 +8127,13 @@
         <v>0</v>
       </c>
       <c r="I27" s="86" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="J27" s="86" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="K27" s="86" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="L27" s="9">
         <v>10</v>
@@ -8146,13 +8149,13 @@
     </row>
     <row r="28" spans="1:15" s="24" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A28" s="10" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="B28" s="10" t="s">
         <v>61</v>
       </c>
       <c r="C28" s="10" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="D28" s="82">
         <v>1</v>
@@ -8170,13 +8173,13 @@
         <v>0</v>
       </c>
       <c r="I28" s="86" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="J28" s="86" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="K28" s="86" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="L28" s="9">
         <v>21</v>
@@ -8192,13 +8195,13 @@
     </row>
     <row r="29" spans="1:15" s="24" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A29" s="10" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="B29" s="10" t="s">
         <v>62</v>
       </c>
       <c r="C29" s="10" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="D29" s="82">
         <v>1</v>
@@ -8216,13 +8219,13 @@
         <v>0</v>
       </c>
       <c r="I29" s="86" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="J29" s="86" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="K29" s="86" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="L29" s="52">
         <f>10*30/7</f>
@@ -8239,13 +8242,13 @@
     </row>
     <row r="30" spans="1:15" s="24" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A30" s="11" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="B30" s="11" t="s">
         <v>59</v>
       </c>
       <c r="C30" s="11" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="D30" s="83">
         <v>1</v>
@@ -8263,13 +8266,13 @@
         <v>1</v>
       </c>
       <c r="I30" s="85" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="J30" s="85" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="K30" s="85" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="L30" s="7">
         <v>5</v>
@@ -8285,13 +8288,13 @@
     </row>
     <row r="31" spans="1:15" s="24" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A31" s="10" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="B31" s="10" t="s">
         <v>60</v>
       </c>
       <c r="C31" s="10" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="D31" s="82">
         <v>1</v>
@@ -8309,13 +8312,13 @@
         <v>0</v>
       </c>
       <c r="I31" s="86" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="J31" s="86" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="K31" s="86" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="L31" s="9">
         <v>10</v>
@@ -8331,13 +8334,13 @@
     </row>
     <row r="32" spans="1:15" s="24" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A32" s="10" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="B32" s="10" t="s">
         <v>61</v>
       </c>
       <c r="C32" s="10" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="D32" s="82">
         <v>1</v>
@@ -8355,13 +8358,13 @@
         <v>0</v>
       </c>
       <c r="I32" s="86" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="J32" s="86" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="K32" s="86" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="L32" s="9">
         <v>21</v>
@@ -8377,13 +8380,13 @@
     </row>
     <row r="33" spans="1:15" s="24" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A33" s="10" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="B33" s="10" t="s">
         <v>62</v>
       </c>
       <c r="C33" s="10" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="D33" s="82">
         <v>1</v>
@@ -8401,13 +8404,13 @@
         <v>0</v>
       </c>
       <c r="I33" s="86" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="J33" s="86" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="K33" s="86" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="L33" s="52">
         <f>10*30/7</f>
@@ -8424,13 +8427,13 @@
     </row>
     <row r="34" spans="1:15" s="24" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A34" s="11" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="B34" s="11" t="s">
         <v>59</v>
       </c>
       <c r="C34" s="11" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="D34" s="83">
         <v>1</v>
@@ -8448,13 +8451,13 @@
         <v>1</v>
       </c>
       <c r="I34" s="85" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="J34" s="85" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="K34" s="85" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="L34" s="7">
         <v>5</v>
@@ -8470,13 +8473,13 @@
     </row>
     <row r="35" spans="1:15" s="24" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A35" s="10" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="B35" s="10" t="s">
         <v>60</v>
       </c>
       <c r="C35" s="10" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="D35" s="82">
         <v>1</v>
@@ -8494,13 +8497,13 @@
         <v>0</v>
       </c>
       <c r="I35" s="86" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="J35" s="86" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="K35" s="86" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="L35" s="9">
         <v>10</v>
@@ -8516,13 +8519,13 @@
     </row>
     <row r="36" spans="1:15" s="24" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A36" s="10" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="B36" s="10" t="s">
         <v>61</v>
       </c>
       <c r="C36" s="10" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="D36" s="82">
         <v>1</v>
@@ -8540,13 +8543,13 @@
         <v>0</v>
       </c>
       <c r="I36" s="86" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="J36" s="86" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="K36" s="86" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="L36" s="9">
         <v>21</v>
@@ -8562,13 +8565,13 @@
     </row>
     <row r="37" spans="1:15" s="24" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A37" s="10" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="B37" s="10" t="s">
         <v>62</v>
       </c>
       <c r="C37" s="10" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="D37" s="82">
         <v>1</v>
@@ -8586,13 +8589,13 @@
         <v>0</v>
       </c>
       <c r="I37" s="86" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="J37" s="86" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="K37" s="86" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="L37" s="52">
         <f>10*30/7</f>
@@ -8609,13 +8612,13 @@
     </row>
     <row r="38" spans="1:15" s="24" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A38" s="11" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="B38" s="11" t="s">
         <v>59</v>
       </c>
       <c r="C38" s="11" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="D38" s="83">
         <v>1</v>
@@ -8633,13 +8636,13 @@
         <v>1</v>
       </c>
       <c r="I38" s="85" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="J38" s="85" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="K38" s="85" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="L38" s="7">
         <v>5</v>
@@ -8655,13 +8658,13 @@
     </row>
     <row r="39" spans="1:15" s="24" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A39" s="10" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="B39" s="10" t="s">
         <v>60</v>
       </c>
       <c r="C39" s="10" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="D39" s="82">
         <v>1</v>
@@ -8679,13 +8682,13 @@
         <v>0</v>
       </c>
       <c r="I39" s="86" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="J39" s="86" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="K39" s="86" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="L39" s="9">
         <v>10</v>
@@ -8701,13 +8704,13 @@
     </row>
     <row r="40" spans="1:15" s="24" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A40" s="10" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="B40" s="10" t="s">
         <v>61</v>
       </c>
       <c r="C40" s="10" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="D40" s="82">
         <v>1</v>
@@ -8725,13 +8728,13 @@
         <v>0</v>
       </c>
       <c r="I40" s="86" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="J40" s="86" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="K40" s="86" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="L40" s="9">
         <v>21</v>
@@ -8747,13 +8750,13 @@
     </row>
     <row r="41" spans="1:15" s="24" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A41" s="12" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="B41" s="12" t="s">
         <v>62</v>
       </c>
       <c r="C41" s="12" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="D41" s="84">
         <v>1</v>
@@ -8771,13 +8774,13 @@
         <v>0</v>
       </c>
       <c r="I41" s="86" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="J41" s="86" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="K41" s="86" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="L41" s="52">
         <f>10*30/7</f>
@@ -8794,13 +8797,13 @@
     </row>
     <row r="42" spans="1:15" s="24" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A42" s="11" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="B42" s="11" t="s">
         <v>59</v>
       </c>
       <c r="C42" s="11" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="D42" s="83">
         <v>1</v>
@@ -8818,13 +8821,13 @@
         <v>1</v>
       </c>
       <c r="I42" s="85" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="J42" s="85" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="K42" s="85" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="L42" s="7">
         <v>5</v>
@@ -8840,13 +8843,13 @@
     </row>
     <row r="43" spans="1:15" s="24" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A43" s="10" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="B43" s="10" t="s">
         <v>60</v>
       </c>
       <c r="C43" s="10" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="D43" s="82">
         <v>1</v>
@@ -8864,13 +8867,13 @@
         <v>0</v>
       </c>
       <c r="I43" s="86" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="J43" s="86" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="K43" s="86" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="L43" s="9">
         <v>10</v>
@@ -8886,13 +8889,13 @@
     </row>
     <row r="44" spans="1:15" s="24" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A44" s="10" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="B44" s="10" t="s">
         <v>61</v>
       </c>
       <c r="C44" s="10" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="D44" s="82">
         <v>1</v>
@@ -8910,13 +8913,13 @@
         <v>0</v>
       </c>
       <c r="I44" s="86" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="J44" s="86" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="K44" s="86" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="L44" s="9">
         <v>21</v>
@@ -8932,13 +8935,13 @@
     </row>
     <row r="45" spans="1:15" s="24" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A45" s="10" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="B45" s="10" t="s">
         <v>62</v>
       </c>
       <c r="C45" s="10" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="D45" s="82">
         <v>1</v>
@@ -8956,13 +8959,13 @@
         <v>0</v>
       </c>
       <c r="I45" s="86" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="J45" s="86" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="K45" s="86" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="L45" s="52">
         <f>10*30/7</f>
@@ -8979,13 +8982,13 @@
     </row>
     <row r="46" spans="1:15" s="24" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A46" s="11" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="B46" s="11" t="s">
         <v>59</v>
       </c>
       <c r="C46" s="11" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="D46" s="83">
         <v>1</v>
@@ -9003,13 +9006,13 @@
         <v>1</v>
       </c>
       <c r="I46" s="85" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="J46" s="85" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="K46" s="85" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="L46" s="7">
         <v>5</v>
@@ -9025,13 +9028,13 @@
     </row>
     <row r="47" spans="1:15" s="24" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A47" s="10" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="B47" s="10" t="s">
         <v>60</v>
       </c>
       <c r="C47" s="10" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="D47" s="82">
         <v>1</v>
@@ -9049,13 +9052,13 @@
         <v>0</v>
       </c>
       <c r="I47" s="86" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="J47" s="86" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="K47" s="86" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="L47" s="9">
         <v>10</v>
@@ -9071,13 +9074,13 @@
     </row>
     <row r="48" spans="1:15" s="24" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A48" s="10" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="B48" s="10" t="s">
         <v>61</v>
       </c>
       <c r="C48" s="10" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="D48" s="82">
         <v>1</v>
@@ -9095,13 +9098,13 @@
         <v>0</v>
       </c>
       <c r="I48" s="86" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="J48" s="86" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="K48" s="86" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="L48" s="9">
         <v>21</v>
@@ -9117,13 +9120,13 @@
     </row>
     <row r="49" spans="1:15" s="24" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A49" s="10" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="B49" s="10" t="s">
         <v>62</v>
       </c>
       <c r="C49" s="10" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="D49" s="82">
         <v>1</v>
@@ -9141,13 +9144,13 @@
         <v>0</v>
       </c>
       <c r="I49" s="86" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="J49" s="86" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="K49" s="86" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="L49" s="52">
         <f>10*30/7</f>
@@ -9170,7 +9173,7 @@
         <v>59</v>
       </c>
       <c r="C50" s="11" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="D50" s="83">
         <v>1</v>
@@ -9188,13 +9191,13 @@
         <v>1</v>
       </c>
       <c r="I50" s="85" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="J50" s="85" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="K50" s="85" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="L50" s="7">
         <v>5</v>
@@ -9216,7 +9219,7 @@
         <v>60</v>
       </c>
       <c r="C51" s="10" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="D51" s="82">
         <v>1</v>
@@ -9234,13 +9237,13 @@
         <v>0</v>
       </c>
       <c r="I51" s="86" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="J51" s="86" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="K51" s="86" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="L51" s="9">
         <v>10</v>
@@ -9262,7 +9265,7 @@
         <v>61</v>
       </c>
       <c r="C52" s="10" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="D52" s="82">
         <v>1</v>
@@ -9280,13 +9283,13 @@
         <v>0</v>
       </c>
       <c r="I52" s="86" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="J52" s="86" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="K52" s="86" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="L52" s="9">
         <v>21</v>
@@ -9308,7 +9311,7 @@
         <v>62</v>
       </c>
       <c r="C53" s="10" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="D53" s="82">
         <v>1</v>
@@ -9326,13 +9329,13 @@
         <v>0</v>
       </c>
       <c r="I53" s="86" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="J53" s="86" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="K53" s="86" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="L53" s="52">
         <f>10*30/7</f>
@@ -9349,13 +9352,13 @@
     </row>
     <row r="54" spans="1:15" s="24" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A54" s="11" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="B54" s="11" t="s">
         <v>59</v>
       </c>
       <c r="C54" s="11" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="D54" s="83">
         <v>1</v>
@@ -9373,13 +9376,13 @@
         <v>1</v>
       </c>
       <c r="I54" s="85" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="J54" s="85" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="K54" s="85" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="L54" s="7">
         <v>5</v>
@@ -9395,13 +9398,13 @@
     </row>
     <row r="55" spans="1:15" s="24" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A55" s="10" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="B55" s="10" t="s">
         <v>60</v>
       </c>
       <c r="C55" s="10" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="D55" s="82">
         <v>1</v>
@@ -9419,13 +9422,13 @@
         <v>0</v>
       </c>
       <c r="I55" s="86" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="J55" s="86" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="K55" s="86" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="L55" s="9">
         <v>10</v>
@@ -9441,13 +9444,13 @@
     </row>
     <row r="56" spans="1:15" s="24" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A56" s="10" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="B56" s="10" t="s">
         <v>61</v>
       </c>
       <c r="C56" s="10" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="D56" s="82">
         <v>1</v>
@@ -9465,13 +9468,13 @@
         <v>0</v>
       </c>
       <c r="I56" s="86" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="J56" s="86" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="K56" s="86" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="L56" s="9">
         <v>21</v>
@@ -9487,13 +9490,13 @@
     </row>
     <row r="57" spans="1:15" s="24" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A57" s="12" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="B57" s="12" t="s">
         <v>62</v>
       </c>
       <c r="C57" s="12" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="D57" s="84">
         <v>1</v>
@@ -9511,13 +9514,13 @@
         <v>0</v>
       </c>
       <c r="I57" s="86" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="J57" s="86" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="K57" s="86" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="L57" s="52">
         <f>10*30/7</f>
@@ -9534,13 +9537,13 @@
     </row>
     <row r="58" spans="1:15" s="24" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A58" s="10" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="B58" s="10" t="s">
         <v>59</v>
       </c>
       <c r="C58" s="10" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="D58" s="82">
         <v>1</v>
@@ -9558,13 +9561,13 @@
         <v>1</v>
       </c>
       <c r="I58" s="85" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="J58" s="85" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="K58" s="85" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="L58" s="7">
         <v>5</v>
@@ -9580,13 +9583,13 @@
     </row>
     <row r="59" spans="1:15" s="24" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A59" s="10" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="B59" s="10" t="s">
         <v>60</v>
       </c>
       <c r="C59" s="10" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="D59" s="82">
         <v>1</v>
@@ -9604,13 +9607,13 @@
         <v>0</v>
       </c>
       <c r="I59" s="86" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="J59" s="86" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="K59" s="86" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="L59" s="9">
         <v>10</v>
@@ -9626,13 +9629,13 @@
     </row>
     <row r="60" spans="1:15" s="24" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A60" s="10" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="B60" s="10" t="s">
         <v>61</v>
       </c>
       <c r="C60" s="10" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="D60" s="82">
         <v>1</v>
@@ -9650,13 +9653,13 @@
         <v>0</v>
       </c>
       <c r="I60" s="86" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="J60" s="86" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="K60" s="86" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="L60" s="9">
         <v>21</v>
@@ -9672,13 +9675,13 @@
     </row>
     <row r="61" spans="1:15" s="24" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A61" s="10" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="B61" s="10" t="s">
         <v>62</v>
       </c>
       <c r="C61" s="10" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="D61" s="82">
         <v>1</v>
@@ -9696,13 +9699,13 @@
         <v>0</v>
       </c>
       <c r="I61" s="86" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="J61" s="86" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="K61" s="86" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="L61" s="52">
         <f>10*30/7</f>
@@ -9719,13 +9722,13 @@
     </row>
     <row r="62" spans="1:15" s="24" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A62" s="11" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="B62" s="11" t="s">
         <v>59</v>
       </c>
       <c r="C62" s="11" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="D62" s="83">
         <v>1</v>
@@ -9743,13 +9746,13 @@
         <v>1</v>
       </c>
       <c r="I62" s="85" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="J62" s="85" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="K62" s="85" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="L62" s="7">
         <v>5</v>
@@ -9765,13 +9768,13 @@
     </row>
     <row r="63" spans="1:15" s="24" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A63" s="10" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="B63" s="10" t="s">
         <v>60</v>
       </c>
       <c r="C63" s="10" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="D63" s="82">
         <v>1</v>
@@ -9789,13 +9792,13 @@
         <v>0</v>
       </c>
       <c r="I63" s="86" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="J63" s="86" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="K63" s="86" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="L63" s="9">
         <v>10</v>
@@ -9811,13 +9814,13 @@
     </row>
     <row r="64" spans="1:15" s="24" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A64" s="10" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="B64" s="10" t="s">
         <v>61</v>
       </c>
       <c r="C64" s="10" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="D64" s="82">
         <v>1</v>
@@ -9835,13 +9838,13 @@
         <v>0</v>
       </c>
       <c r="I64" s="86" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="J64" s="86" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="K64" s="86" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="L64" s="9">
         <v>21</v>
@@ -9857,13 +9860,13 @@
     </row>
     <row r="65" spans="1:15" s="43" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A65" s="12" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="B65" s="12" t="s">
         <v>62</v>
       </c>
       <c r="C65" s="12" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="D65" s="84">
         <v>1</v>
@@ -9881,13 +9884,13 @@
         <v>0</v>
       </c>
       <c r="I65" s="86" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="J65" s="86" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="K65" s="86" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="L65" s="52">
         <f>10*30/7</f>
@@ -9910,7 +9913,7 @@
         <v>59</v>
       </c>
       <c r="C66" s="11" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="D66" s="83">
         <v>1</v>
@@ -9928,13 +9931,13 @@
         <v>1</v>
       </c>
       <c r="I66" s="85" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="J66" s="85" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="K66" s="85" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="L66" s="7">
         <v>1</v>
@@ -9958,7 +9961,7 @@
         <v>60</v>
       </c>
       <c r="C67" s="10" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="D67" s="82">
         <v>1</v>
@@ -9976,13 +9979,13 @@
         <v>0.6</v>
       </c>
       <c r="I67" s="86" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="J67" s="86" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="K67" s="86" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="L67" s="9">
         <v>3</v>
@@ -10006,7 +10009,7 @@
         <v>61</v>
       </c>
       <c r="C68" s="10" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="D68" s="82">
         <v>1</v>
@@ -10024,13 +10027,13 @@
         <v>0.2</v>
       </c>
       <c r="I68" s="86" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="J68" s="86" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="K68" s="86" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="L68" s="9">
         <v>7</v>
@@ -10054,7 +10057,7 @@
         <v>62</v>
       </c>
       <c r="C69" s="10" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="D69" s="82">
         <v>1</v>
@@ -10072,13 +10075,13 @@
         <v>0</v>
       </c>
       <c r="I69" s="86" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="J69" s="86" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="K69" s="86" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="L69" s="9">
         <v>30</v>
@@ -10102,7 +10105,7 @@
         <v>59</v>
       </c>
       <c r="C70" s="90" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="D70" s="91">
         <v>1</v>
@@ -10120,13 +10123,13 @@
         <v>1</v>
       </c>
       <c r="I70" s="93" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="J70" s="93" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="K70" s="93" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="L70" s="94">
         <v>1</v>
@@ -10148,7 +10151,7 @@
         <v>60</v>
       </c>
       <c r="C71" s="95" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="D71" s="96">
         <v>1</v>
@@ -10166,13 +10169,13 @@
         <v>1</v>
       </c>
       <c r="I71" s="98" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="J71" s="98" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="K71" s="98" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="L71" s="99">
         <v>1</v>
@@ -10194,7 +10197,7 @@
         <v>61</v>
       </c>
       <c r="C72" s="95" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="D72" s="96">
         <v>1</v>
@@ -10212,13 +10215,13 @@
         <v>1</v>
       </c>
       <c r="I72" s="98" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="J72" s="98" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="K72" s="98" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="L72" s="99">
         <v>1</v>
@@ -10240,7 +10243,7 @@
         <v>62</v>
       </c>
       <c r="C73" s="100" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="D73" s="101">
         <v>1</v>
@@ -10258,13 +10261,13 @@
         <v>1</v>
       </c>
       <c r="I73" s="103" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="J73" s="103" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="K73" s="103" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="L73" s="104">
         <v>1</v>
@@ -10280,13 +10283,13 @@
     </row>
     <row r="74" spans="1:15" s="24" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A74" s="90" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="B74" s="90" t="s">
         <v>59</v>
       </c>
       <c r="C74" s="90" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="D74" s="91">
         <v>1</v>
@@ -10304,13 +10307,13 @@
         <v>1</v>
       </c>
       <c r="I74" s="93" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="J74" s="93" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="K74" s="93" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="L74" s="94">
         <v>1</v>
@@ -10326,13 +10329,13 @@
     </row>
     <row r="75" spans="1:15" s="24" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A75" s="95" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="B75" s="95" t="s">
         <v>60</v>
       </c>
       <c r="C75" s="95" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="D75" s="96">
         <v>1</v>
@@ -10350,13 +10353,13 @@
         <v>1</v>
       </c>
       <c r="I75" s="98" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="J75" s="98" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="K75" s="98" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="L75" s="99">
         <v>1</v>
@@ -10372,13 +10375,13 @@
     </row>
     <row r="76" spans="1:15" s="24" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A76" s="95" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="B76" s="95" t="s">
         <v>61</v>
       </c>
       <c r="C76" s="95" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="D76" s="96">
         <v>1</v>
@@ -10396,13 +10399,13 @@
         <v>1</v>
       </c>
       <c r="I76" s="98" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="J76" s="98" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="K76" s="98" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="L76" s="99">
         <v>1</v>
@@ -10418,13 +10421,13 @@
     </row>
     <row r="77" spans="1:15" s="24" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A77" s="100" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="B77" s="100" t="s">
         <v>62</v>
       </c>
       <c r="C77" s="100" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="D77" s="101">
         <v>1</v>
@@ -10442,13 +10445,13 @@
         <v>1</v>
       </c>
       <c r="I77" s="103" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="J77" s="103" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="K77" s="103" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="L77" s="104">
         <v>1</v>
@@ -10500,12 +10503,12 @@
         <v>19</v>
       </c>
       <c r="C1" s="58" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
     </row>
     <row r="2" spans="1:3" s="24" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="8" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="B2" s="11" t="s">
         <v>59</v>
@@ -10516,7 +10519,7 @@
     </row>
     <row r="3" spans="1:3" s="24" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="8" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="B3" s="10" t="s">
         <v>60</v>
@@ -10527,7 +10530,7 @@
     </row>
     <row r="4" spans="1:3" s="24" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="8" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="B4" s="10" t="s">
         <v>61</v>
@@ -10538,7 +10541,7 @@
     </row>
     <row r="5" spans="1:3" s="24" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="8" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="B5" s="10" t="s">
         <v>62</v>
@@ -10549,7 +10552,7 @@
     </row>
     <row r="6" spans="1:3" s="24" customFormat="1" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A6" s="11" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="B6" s="11" t="s">
         <v>59</v>
@@ -10560,7 +10563,7 @@
     </row>
     <row r="7" spans="1:3" s="24" customFormat="1" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A7" s="10" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="B7" s="10" t="s">
         <v>60</v>
@@ -10571,7 +10574,7 @@
     </row>
     <row r="8" spans="1:3" s="24" customFormat="1" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A8" s="10" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="B8" s="10" t="s">
         <v>61</v>
@@ -10582,7 +10585,7 @@
     </row>
     <row r="9" spans="1:3" s="24" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="12" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="B9" s="12" t="s">
         <v>62</v>
@@ -10593,7 +10596,7 @@
     </row>
     <row r="10" spans="1:3" s="43" customFormat="1" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A10" s="10" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="B10" s="10" t="s">
         <v>59</v>
@@ -10604,7 +10607,7 @@
     </row>
     <row r="11" spans="1:3" s="24" customFormat="1" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A11" s="10" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="B11" s="10" t="s">
         <v>60</v>
@@ -10615,7 +10618,7 @@
     </row>
     <row r="12" spans="1:3" s="24" customFormat="1" ht="51" x14ac:dyDescent="0.25">
       <c r="A12" s="10" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="B12" s="10" t="s">
         <v>61</v>
@@ -10626,7 +10629,7 @@
     </row>
     <row r="13" spans="1:3" s="24" customFormat="1" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A13" s="10" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="B13" s="10" t="s">
         <v>62</v>
@@ -10637,7 +10640,7 @@
     </row>
     <row r="14" spans="1:3" s="24" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A14" s="11" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="B14" s="11" t="s">
         <v>59</v>
@@ -10648,7 +10651,7 @@
     </row>
     <row r="15" spans="1:3" s="24" customFormat="1" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A15" s="10" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="B15" s="10" t="s">
         <v>60</v>
@@ -10659,7 +10662,7 @@
     </row>
     <row r="16" spans="1:3" s="24" customFormat="1" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A16" s="10" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="B16" s="10" t="s">
         <v>61</v>
@@ -10670,7 +10673,7 @@
     </row>
     <row r="17" spans="1:3" s="24" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A17" s="10" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="B17" s="10" t="s">
         <v>62</v>
@@ -10681,7 +10684,7 @@
     </row>
     <row r="18" spans="1:3" s="24" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A18" s="11" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="B18" s="11" t="s">
         <v>59</v>
@@ -10692,7 +10695,7 @@
     </row>
     <row r="19" spans="1:3" s="24" customFormat="1" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A19" s="10" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="B19" s="10" t="s">
         <v>60</v>
@@ -10703,7 +10706,7 @@
     </row>
     <row r="20" spans="1:3" s="24" customFormat="1" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A20" s="10" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="B20" s="10" t="s">
         <v>61</v>
@@ -10714,7 +10717,7 @@
     </row>
     <row r="21" spans="1:3" s="24" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A21" s="10" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="B21" s="10" t="s">
         <v>62</v>
@@ -10725,7 +10728,7 @@
     </row>
     <row r="22" spans="1:3" s="24" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A22" s="11" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="B22" s="11" t="s">
         <v>59</v>
@@ -10736,7 +10739,7 @@
     </row>
     <row r="23" spans="1:3" s="24" customFormat="1" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A23" s="10" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="B23" s="10" t="s">
         <v>60</v>
@@ -10747,7 +10750,7 @@
     </row>
     <row r="24" spans="1:3" s="24" customFormat="1" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A24" s="10" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="B24" s="10" t="s">
         <v>61</v>
@@ -10758,7 +10761,7 @@
     </row>
     <row r="25" spans="1:3" s="24" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A25" s="10" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="B25" s="10" t="s">
         <v>62</v>
@@ -10769,7 +10772,7 @@
     </row>
     <row r="26" spans="1:3" s="24" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A26" s="11" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="B26" s="11" t="s">
         <v>59</v>
@@ -10780,7 +10783,7 @@
     </row>
     <row r="27" spans="1:3" s="24" customFormat="1" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A27" s="10" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="B27" s="10" t="s">
         <v>60</v>
@@ -10791,7 +10794,7 @@
     </row>
     <row r="28" spans="1:3" s="24" customFormat="1" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A28" s="10" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="B28" s="10" t="s">
         <v>61</v>
@@ -10802,7 +10805,7 @@
     </row>
     <row r="29" spans="1:3" s="24" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A29" s="10" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="B29" s="10" t="s">
         <v>62</v>
@@ -10813,7 +10816,7 @@
     </row>
     <row r="30" spans="1:3" s="24" customFormat="1" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A30" s="11" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="B30" s="11" t="s">
         <v>59</v>
@@ -10824,7 +10827,7 @@
     </row>
     <row r="31" spans="1:3" s="24" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A31" s="10" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="B31" s="10" t="s">
         <v>60</v>
@@ -10835,7 +10838,7 @@
     </row>
     <row r="32" spans="1:3" s="24" customFormat="1" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A32" s="10" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="B32" s="10" t="s">
         <v>61</v>
@@ -10846,7 +10849,7 @@
     </row>
     <row r="33" spans="1:3" s="24" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A33" s="10" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="B33" s="10" t="s">
         <v>62</v>
@@ -10857,7 +10860,7 @@
     </row>
     <row r="34" spans="1:3" s="24" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A34" s="11" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="B34" s="11" t="s">
         <v>59</v>
@@ -10868,7 +10871,7 @@
     </row>
     <row r="35" spans="1:3" s="24" customFormat="1" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A35" s="10" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="B35" s="10" t="s">
         <v>60</v>
@@ -10879,7 +10882,7 @@
     </row>
     <row r="36" spans="1:3" s="24" customFormat="1" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A36" s="10" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="B36" s="10" t="s">
         <v>61</v>
@@ -10890,7 +10893,7 @@
     </row>
     <row r="37" spans="1:3" s="24" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A37" s="12" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="B37" s="12" t="s">
         <v>62</v>
@@ -10901,7 +10904,7 @@
     </row>
     <row r="38" spans="1:3" s="24" customFormat="1" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A38" s="11" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="B38" s="11" t="s">
         <v>59</v>
@@ -10912,7 +10915,7 @@
     </row>
     <row r="39" spans="1:3" s="24" customFormat="1" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A39" s="10" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="B39" s="10" t="s">
         <v>60</v>
@@ -10923,7 +10926,7 @@
     </row>
     <row r="40" spans="1:3" s="24" customFormat="1" ht="51" x14ac:dyDescent="0.25">
       <c r="A40" s="10" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="B40" s="10" t="s">
         <v>61</v>
@@ -10934,7 +10937,7 @@
     </row>
     <row r="41" spans="1:3" s="24" customFormat="1" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A41" s="12" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="B41" s="12" t="s">
         <v>62</v>
@@ -10945,7 +10948,7 @@
     </row>
     <row r="42" spans="1:3" s="24" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A42" s="11" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="B42" s="11" t="s">
         <v>59</v>
@@ -10956,7 +10959,7 @@
     </row>
     <row r="43" spans="1:3" s="24" customFormat="1" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A43" s="10" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="B43" s="10" t="s">
         <v>60</v>
@@ -10967,7 +10970,7 @@
     </row>
     <row r="44" spans="1:3" s="24" customFormat="1" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A44" s="10" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="B44" s="10" t="s">
         <v>61</v>
@@ -10978,7 +10981,7 @@
     </row>
     <row r="45" spans="1:3" s="24" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A45" s="10" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="B45" s="10" t="s">
         <v>62</v>
@@ -10989,7 +10992,7 @@
     </row>
     <row r="46" spans="1:3" s="24" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A46" s="11" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="B46" s="11" t="s">
         <v>59</v>
@@ -11000,7 +11003,7 @@
     </row>
     <row r="47" spans="1:3" s="24" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A47" s="10" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="B47" s="10" t="s">
         <v>60</v>
@@ -11011,7 +11014,7 @@
     </row>
     <row r="48" spans="1:3" s="24" customFormat="1" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A48" s="10" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="B48" s="10" t="s">
         <v>61</v>
@@ -11022,7 +11025,7 @@
     </row>
     <row r="49" spans="1:3" s="24" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A49" s="10" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="B49" s="10" t="s">
         <v>62</v>
@@ -11077,7 +11080,7 @@
     </row>
     <row r="54" spans="1:3" s="24" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A54" s="11" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="B54" s="11" t="s">
         <v>59</v>
@@ -11088,7 +11091,7 @@
     </row>
     <row r="55" spans="1:3" s="24" customFormat="1" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A55" s="10" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="B55" s="10" t="s">
         <v>60</v>
@@ -11099,7 +11102,7 @@
     </row>
     <row r="56" spans="1:3" s="24" customFormat="1" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A56" s="10" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="B56" s="10" t="s">
         <v>61</v>
@@ -11110,7 +11113,7 @@
     </row>
     <row r="57" spans="1:3" s="24" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A57" s="10" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="B57" s="10" t="s">
         <v>62</v>
@@ -11121,7 +11124,7 @@
     </row>
     <row r="58" spans="1:3" s="24" customFormat="1" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A58" s="11" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="B58" s="11" t="s">
         <v>59</v>
@@ -11132,7 +11135,7 @@
     </row>
     <row r="59" spans="1:3" s="24" customFormat="1" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A59" s="10" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="B59" s="10" t="s">
         <v>60</v>
@@ -11143,7 +11146,7 @@
     </row>
     <row r="60" spans="1:3" s="24" customFormat="1" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A60" s="10" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="B60" s="10" t="s">
         <v>61</v>
@@ -11154,7 +11157,7 @@
     </row>
     <row r="61" spans="1:3" s="24" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A61" s="10" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="B61" s="10" t="s">
         <v>62</v>
@@ -11165,7 +11168,7 @@
     </row>
     <row r="62" spans="1:3" s="24" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A62" s="11" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="B62" s="11" t="s">
         <v>59</v>
@@ -11176,7 +11179,7 @@
     </row>
     <row r="63" spans="1:3" s="24" customFormat="1" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A63" s="10" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="B63" s="10" t="s">
         <v>60</v>
@@ -11187,7 +11190,7 @@
     </row>
     <row r="64" spans="1:3" s="24" customFormat="1" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A64" s="10" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="B64" s="10" t="s">
         <v>61</v>
@@ -11198,7 +11201,7 @@
     </row>
     <row r="65" spans="1:3" s="43" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A65" s="10" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="B65" s="10" t="s">
         <v>62</v>
@@ -11215,7 +11218,7 @@
         <v>59</v>
       </c>
       <c r="C66" s="14" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
     </row>
     <row r="67" spans="1:3" s="24" customFormat="1" x14ac:dyDescent="0.25">
@@ -11226,7 +11229,7 @@
         <v>60</v>
       </c>
       <c r="C67" s="14" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
     </row>
     <row r="68" spans="1:3" s="24" customFormat="1" x14ac:dyDescent="0.25">
@@ -11237,7 +11240,7 @@
         <v>61</v>
       </c>
       <c r="C68" s="14" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
     </row>
     <row r="69" spans="1:3" s="24" customFormat="1" x14ac:dyDescent="0.25">
@@ -11248,7 +11251,7 @@
         <v>62</v>
       </c>
       <c r="C69" s="14" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
     </row>
     <row r="70" spans="1:3" s="24" customFormat="1" x14ac:dyDescent="0.25">
@@ -11259,7 +11262,7 @@
         <v>59</v>
       </c>
       <c r="C70" s="14" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
     </row>
     <row r="71" spans="1:3" s="24" customFormat="1" x14ac:dyDescent="0.25">
@@ -11270,7 +11273,7 @@
         <v>60</v>
       </c>
       <c r="C71" s="14" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
     </row>
     <row r="72" spans="1:3" s="24" customFormat="1" x14ac:dyDescent="0.25">
@@ -11281,7 +11284,7 @@
         <v>61</v>
       </c>
       <c r="C72" s="14" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
     </row>
     <row r="73" spans="1:3" s="24" customFormat="1" x14ac:dyDescent="0.25">
@@ -11292,51 +11295,51 @@
         <v>62</v>
       </c>
       <c r="C73" s="14" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
     </row>
     <row r="74" spans="1:3" s="24" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A74" s="90" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="B74" s="90" t="s">
         <v>59</v>
       </c>
       <c r="C74" s="14" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
     </row>
     <row r="75" spans="1:3" s="24" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A75" s="95" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="B75" s="95" t="s">
         <v>60</v>
       </c>
       <c r="C75" s="14" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
     </row>
     <row r="76" spans="1:3" s="24" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A76" s="95" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="B76" s="95" t="s">
         <v>61</v>
       </c>
       <c r="C76" s="14" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
     </row>
     <row r="77" spans="1:3" s="24" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A77" s="100" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="B77" s="100" t="s">
         <v>62</v>
       </c>
       <c r="C77" s="14" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
     </row>
   </sheetData>
@@ -11565,7 +11568,7 @@
         <v>76</v>
       </c>
       <c r="J9" s="19" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
     </row>
     <row r="10" spans="1:10" s="24" customFormat="1" ht="25.5" x14ac:dyDescent="0.25">
@@ -11931,7 +11934,7 @@
         <v>88</v>
       </c>
       <c r="J21" s="26" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
     </row>
     <row r="22" spans="1:10" s="24" customFormat="1" ht="38.25" x14ac:dyDescent="0.25">
@@ -12304,7 +12307,7 @@
         <v>161</v>
       </c>
       <c r="J33" s="26" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
     </row>
     <row r="34" spans="1:10" s="24" customFormat="1" ht="38.25" x14ac:dyDescent="0.25">
@@ -13708,7 +13711,7 @@
         <v>72</v>
       </c>
       <c r="J5" s="19" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
     </row>
     <row r="6" spans="1:10" s="24" customFormat="1" x14ac:dyDescent="0.25">
@@ -13740,7 +13743,7 @@
         <v>73</v>
       </c>
       <c r="J6" s="19" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
     </row>
     <row r="7" spans="1:10" s="24" customFormat="1" ht="25.5" x14ac:dyDescent="0.25">
@@ -13772,7 +13775,7 @@
         <v>74</v>
       </c>
       <c r="J7" s="19" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
     </row>
     <row r="8" spans="1:10" s="24" customFormat="1" x14ac:dyDescent="0.25">
@@ -13805,7 +13808,7 @@
         <v>75</v>
       </c>
       <c r="J8" s="19" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
     </row>
     <row r="9" spans="1:10" s="24" customFormat="1" ht="38.25" x14ac:dyDescent="0.25">
@@ -13837,7 +13840,7 @@
         <v>76</v>
       </c>
       <c r="J9" s="26" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
     </row>
     <row r="10" spans="1:10" s="24" customFormat="1" ht="25.5" x14ac:dyDescent="0.25">
@@ -14209,7 +14212,7 @@
         <v>88</v>
       </c>
       <c r="J21" s="26" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
     </row>
     <row r="22" spans="1:10" s="24" customFormat="1" ht="38.25" x14ac:dyDescent="0.25">
@@ -14582,7 +14585,7 @@
         <v>161</v>
       </c>
       <c r="J33" s="26" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
     </row>
     <row r="34" spans="1:10" s="24" customFormat="1" ht="38.25" x14ac:dyDescent="0.25">

</xml_diff>